<commit_message>
Add basic writing to template - header and line items
</commit_message>
<xml_diff>
--- a/templates/base_invoice_template.xlsx
+++ b/templates/base_invoice_template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/svetlinstoyanov/Dev/Projects/erp_data_parser/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE912239-75D8-9C48-914D-9E386098A9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0281B7EC-E083-7E4C-B855-4875026028D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Фактура</t>
   </si>
@@ -152,19 +165,16 @@
   </si>
   <si>
     <t>Отговарящ за операцията</t>
-  </si>
-  <si>
-    <t>Програмен продукт Microinvest Склад Pro, тел. 0700 44 700, http://www.microinvest.net</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -233,13 +243,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -301,7 +304,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -311,6 +314,12 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -323,38 +332,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
@@ -362,11 +374,8 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,14 +909,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B1:AH46"/>
+  <dimension ref="C1:AG65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showOutlineSymbols="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" showOutlineSymbols="0" zoomScale="144" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -950,166 +959,166 @@
   <sheetData>
     <row r="1" spans="3:33" ht="26.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="3:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
     <row r="3" spans="3:33" ht="0.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
     </row>
     <row r="4" spans="3:33" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
     </row>
     <row r="5" spans="3:33" ht="22.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="6" spans="3:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="K6" s="5" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="K6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="6" t="s">
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="3:33" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="8" spans="3:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="9" spans="3:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="7"/>
-      <c r="AE9" s="7"/>
-      <c r="AF9" s="7"/>
-      <c r="AG9" s="7"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
     </row>
     <row r="10" spans="3:33" ht="3.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="11" spans="3:33" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="T11" s="8" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="T11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="8"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
     </row>
     <row r="12" spans="3:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C12" s="9" t="s">
@@ -1117,10 +1126,29 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
       <c r="T12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="U12" s="9"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
     </row>
     <row r="13" spans="3:33" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C13" s="9" t="s">
@@ -1128,22 +1156,80 @@
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
       <c r="T13" s="9" t="s">
         <v>11</v>
       </c>
       <c r="U13" s="9"/>
-    </row>
-    <row r="14" spans="3:33" ht="0.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+    </row>
+    <row r="14" spans="3:33" ht="0.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+    </row>
     <row r="15" spans="3:33" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
       <c r="T15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="U15" s="9"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="4"/>
     </row>
     <row r="16" spans="3:33" ht="13" x14ac:dyDescent="0.15">
       <c r="C16" s="9" t="s">
@@ -1151,10 +1237,29 @@
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
       <c r="T16" s="9" t="s">
         <v>13</v>
       </c>
       <c r="U16" s="9"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
     </row>
     <row r="17" spans="3:33" ht="13" x14ac:dyDescent="0.15">
       <c r="C17" s="9" t="s">
@@ -1163,10 +1268,29 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
       <c r="T17" s="9" t="s">
         <v>14</v>
       </c>
       <c r="U17" s="9"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
     </row>
     <row r="18" spans="3:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C18" s="9" t="s">
@@ -1174,10 +1298,29 @@
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
       <c r="T18" s="9" t="s">
         <v>15</v>
       </c>
       <c r="U18" s="9"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
     </row>
     <row r="19" spans="3:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C19" s="9" t="s">
@@ -1187,6 +1330,15 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="3:33" ht="13" x14ac:dyDescent="0.15">
       <c r="C20" s="9" t="s">
@@ -1196,156 +1348,183 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="3:33" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="22" spans="3:33" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="G22" s="10" t="s">
+      <c r="E22" s="12"/>
+      <c r="G22" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10" t="s">
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10" t="s">
+      <c r="V22" s="12"/>
+      <c r="W22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="X22" s="10"/>
-      <c r="Y22" s="10"/>
-      <c r="Z22" s="10"/>
-      <c r="AA22" s="10" t="s">
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB22" s="10"/>
-      <c r="AC22" s="11" t="s">
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AD22" s="11"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="12" t="s">
+      <c r="AD22" s="19"/>
+      <c r="AE22" s="19"/>
+      <c r="AF22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AG22" s="12"/>
-    </row>
-    <row r="23" spans="3:33" ht="2.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" spans="3:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C24" s="2">
+      <c r="AG22" s="13"/>
+    </row>
+    <row r="23" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C23" s="2">
         <v>1</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="G23" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="14" t="s">
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="V24" s="14"/>
-      <c r="W24" s="15">
+      <c r="V23" s="15"/>
+      <c r="W23" s="16">
         <v>1</v>
       </c>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
-      <c r="AA24" s="16">
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="17">
         <v>1</v>
       </c>
-      <c r="AB24" s="16"/>
-      <c r="AC24" s="17">
+      <c r="AB23" s="17"/>
+      <c r="AC23" s="18">
         <v>20</v>
       </c>
-      <c r="AD24" s="17"/>
-      <c r="AE24" s="17"/>
-      <c r="AF24" s="16">
+      <c r="AD23" s="18"/>
+      <c r="AE23" s="18"/>
+      <c r="AF23" s="17">
         <v>1</v>
       </c>
-      <c r="AG24" s="16"/>
-    </row>
-    <row r="25" spans="3:33" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" spans="3:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="X26" s="18" t="s">
+      <c r="AG23" s="17"/>
+    </row>
+    <row r="24" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X26" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="Y26" s="18"/>
-      <c r="Z26" s="18"/>
-      <c r="AA26" s="18"/>
-      <c r="AB26" s="18"/>
-      <c r="AC26" s="18"/>
-      <c r="AE26" s="19">
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="21"/>
+      <c r="AE26" s="22">
         <v>1</v>
       </c>
-      <c r="AF26" s="19"/>
-      <c r="AG26" s="19"/>
-    </row>
-    <row r="27" spans="3:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="X27" s="18" t="s">
+      <c r="AF26" s="22"/>
+      <c r="AG26" s="22"/>
+    </row>
+    <row r="27" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X27" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Y27" s="18"/>
-      <c r="Z27" s="18"/>
-      <c r="AA27" s="18"/>
-      <c r="AB27" s="18"/>
-      <c r="AC27" s="18"/>
-      <c r="AE27" s="19">
+      <c r="Y27" s="21"/>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="21"/>
+      <c r="AB27" s="21"/>
+      <c r="AC27" s="21"/>
+      <c r="AE27" s="22">
         <v>0.2</v>
       </c>
-      <c r="AF27" s="19"/>
-      <c r="AG27" s="19"/>
-    </row>
-    <row r="28" spans="3:33" ht="0.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="3:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="X29" s="18" t="s">
+      <c r="AF27" s="22"/>
+      <c r="AG27" s="22"/>
+    </row>
+    <row r="28" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X28" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="Y29" s="18"/>
-      <c r="Z29" s="18"/>
-      <c r="AA29" s="18"/>
-      <c r="AB29" s="18"/>
-      <c r="AC29" s="18"/>
-      <c r="AE29" s="19">
+      <c r="Y28" s="21"/>
+      <c r="Z28" s="21"/>
+      <c r="AA28" s="21"/>
+      <c r="AB28" s="21"/>
+      <c r="AC28" s="21"/>
+      <c r="AE28" s="22">
         <v>1.2</v>
       </c>
-      <c r="AF29" s="19"/>
-      <c r="AG29" s="19"/>
-    </row>
-    <row r="30" spans="3:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="3:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="22"/>
+    </row>
+    <row r="29" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+    </row>
+    <row r="31" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C31" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
@@ -1355,15 +1534,26 @@
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
-    </row>
-    <row r="32" spans="3:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="C32" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="20" t="s">
-        <v>34</v>
-      </c>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="20"/>
+      <c r="AA31" s="20"/>
+      <c r="AB31" s="20"/>
+      <c r="AC31" s="20"/>
+      <c r="AD31" s="20"/>
+    </row>
+    <row r="32" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -1390,11 +1580,17 @@
       <c r="AC32" s="20"/>
       <c r="AD32" s="20"/>
     </row>
-    <row r="33" spans="2:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
+    <row r="33" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C33" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="20" t="s">
+        <v>5</v>
+      </c>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
@@ -1402,220 +1598,190 @@
       <c r="M33" s="20"/>
       <c r="N33" s="20"/>
       <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
-      <c r="U33" s="20"/>
-      <c r="V33" s="20"/>
-      <c r="W33" s="20"/>
-      <c r="X33" s="20"/>
-      <c r="Y33" s="20"/>
-      <c r="Z33" s="20"/>
-      <c r="AA33" s="20"/>
-      <c r="AB33" s="20"/>
-      <c r="AC33" s="20"/>
-      <c r="AD33" s="20"/>
-    </row>
-    <row r="34" spans="2:34" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="35" spans="2:34" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="36" spans="2:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C34" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C36" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-    </row>
-    <row r="37" spans="2:34" ht="13" x14ac:dyDescent="0.15">
+      <c r="M36" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Z36" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA36" s="9"/>
+    </row>
+    <row r="37" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C37" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-    </row>
-    <row r="38" spans="2:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="39" spans="2:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C39" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="9"/>
-      <c r="M39" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="M37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Z37" s="9"/>
+      <c r="AA37" s="9"/>
+    </row>
+    <row r="38" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Z38" s="9"/>
+      <c r="AA38" s="9"/>
+    </row>
+    <row r="39" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
-      <c r="Z39" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA39" s="9"/>
-    </row>
-    <row r="40" spans="2:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q39" s="23"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="23"/>
+      <c r="V39" s="23"/>
+      <c r="W39" s="23"/>
+    </row>
+    <row r="40" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C40" s="9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D40" s="9"/>
-      <c r="M40" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Z40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="Z40" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="AA40" s="9"/>
-    </row>
-    <row r="41" spans="2:34" ht="0.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M41" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Z41" s="9"/>
-      <c r="AA41" s="9"/>
-    </row>
-    <row r="42" spans="2:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-    </row>
-    <row r="43" spans="2:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="C43" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="Z43" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA43" s="9"/>
-      <c r="AB43" s="9"/>
-      <c r="AC43" s="9"/>
-      <c r="AD43" s="9"/>
-      <c r="AE43" s="9"/>
-      <c r="AF43" s="9"/>
-    </row>
-    <row r="44" spans="2:34" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="45" spans="2:34" ht="325.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="21"/>
-      <c r="M46" s="21"/>
-      <c r="N46" s="21"/>
-      <c r="O46" s="21"/>
-      <c r="P46" s="21"/>
-      <c r="Q46" s="21"/>
-      <c r="R46" s="21"/>
-      <c r="S46" s="21"/>
-      <c r="T46" s="21"/>
-      <c r="U46" s="21"/>
-      <c r="V46" s="21"/>
-      <c r="W46" s="21"/>
-      <c r="X46" s="21"/>
-      <c r="Y46" s="21"/>
-      <c r="Z46" s="21"/>
-      <c r="AA46" s="21"/>
-      <c r="AB46" s="21"/>
-      <c r="AC46" s="21"/>
-      <c r="AD46" s="21"/>
-      <c r="AE46" s="21"/>
-      <c r="AG46" s="17">
-        <v>1</v>
-      </c>
-      <c r="AH46" s="17"/>
-    </row>
+      <c r="AB40" s="9"/>
+      <c r="AC40" s="9"/>
+      <c r="AD40" s="9"/>
+      <c r="AE40" s="9"/>
+      <c r="AF40" s="9"/>
+    </row>
+    <row r="41" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="53" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="55" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="56" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="57" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="59" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="C43:H43"/>
-    <mergeCell ref="Z43:AF43"/>
-    <mergeCell ref="B46:AE46"/>
-    <mergeCell ref="AG46:AH46"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="M39:P39"/>
-    <mergeCell ref="Z39:AA41"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="M40:P40"/>
-    <mergeCell ref="M41:P42"/>
+  <mergeCells count="74">
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="Z40:AF40"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="M36:P36"/>
+    <mergeCell ref="Z36:AA38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="M38:P39"/>
+    <mergeCell ref="Q39:W39"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:M30"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:M31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:AD33"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="H36:O36"/>
+    <mergeCell ref="E31:AD32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H33:O33"/>
     <mergeCell ref="X26:AC26"/>
     <mergeCell ref="AE26:AG26"/>
     <mergeCell ref="X27:AC27"/>
     <mergeCell ref="AE27:AG27"/>
-    <mergeCell ref="X29:AC29"/>
-    <mergeCell ref="AE29:AG29"/>
+    <mergeCell ref="X28:AC28"/>
+    <mergeCell ref="AE28:AG28"/>
+    <mergeCell ref="W22:Z22"/>
+    <mergeCell ref="AA22:AB22"/>
     <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="G24:T24"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="W24:Z24"/>
-    <mergeCell ref="AA24:AB24"/>
-    <mergeCell ref="AC24:AE24"/>
-    <mergeCell ref="AF24:AG24"/>
+    <mergeCell ref="G23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:Z23"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="AC23:AE23"/>
+    <mergeCell ref="AF23:AG23"/>
+    <mergeCell ref="AC22:AE22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="G22:T22"/>
     <mergeCell ref="U22:V22"/>
-    <mergeCell ref="W22:Z22"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="AC22:AE22"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="I19:Q19"/>
+    <mergeCell ref="I20:Q20"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="T18:U18"/>
     <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="I18:Q18"/>
+    <mergeCell ref="I12:Q12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="T13:U13"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="T15:U15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="T16:U16"/>
+    <mergeCell ref="X13:AG13"/>
+    <mergeCell ref="X15:AG15"/>
+    <mergeCell ref="X16:AG16"/>
+    <mergeCell ref="X17:AG17"/>
+    <mergeCell ref="I17:Q17"/>
+    <mergeCell ref="I16:Q16"/>
+    <mergeCell ref="I15:Q15"/>
+    <mergeCell ref="I13:Q13"/>
+    <mergeCell ref="X18:AG18"/>
+    <mergeCell ref="C2:S3"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="T17:U17"/>
     <mergeCell ref="C9:S9"/>
     <mergeCell ref="T9:AG9"/>
     <mergeCell ref="C11:R11"/>
     <mergeCell ref="T11:AG11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="T12:U12"/>
-    <mergeCell ref="C2:S3"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="X12:AG12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Merge cells after new rows are inserted
</commit_message>
<xml_diff>
--- a/templates/base_invoice_template.xlsx
+++ b/templates/base_invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/svetlinstoyanov/Dev/Projects/erp_data_parser/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0281B7EC-E083-7E4C-B855-4875026028D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606B4442-E934-D643-AF27-CDBDC8BAF54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -318,6 +318,45 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -332,50 +371,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,7 +914,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="C1:AG65"/>
+  <dimension ref="C1:AG64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showOutlineSymbols="0" zoomScale="144" workbookViewId="0"/>
   </sheetViews>
@@ -959,226 +959,226 @@
   <sheetData>
     <row r="1" spans="3:33" ht="26.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="3:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
     </row>
     <row r="3" spans="3:33" ht="0.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
     </row>
     <row r="4" spans="3:33" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
     </row>
     <row r="5" spans="3:33" ht="22.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="6" spans="3:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="K6" s="7" t="s">
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="K6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="8" t="s">
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
     </row>
     <row r="7" spans="3:33" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="8" spans="3:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="9" spans="3:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="10"/>
-      <c r="AB9" s="10"/>
-      <c r="AC9" s="10"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
     </row>
     <row r="10" spans="3:33" ht="3.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="11" spans="3:33" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="T11" s="11" t="s">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="T11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="23"/>
+      <c r="AE11" s="23"/>
+      <c r="AF11" s="23"/>
+      <c r="AG11" s="23"/>
     </row>
     <row r="12" spans="3:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="T12" s="9" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="T12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="U12" s="9"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
-      <c r="AC12" s="4"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
-      <c r="AG12" s="4"/>
+      <c r="U12" s="5"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+      <c r="AF12" s="17"/>
+      <c r="AG12" s="17"/>
     </row>
     <row r="13" spans="3:33" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="T13" s="9" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="T13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="U13" s="9"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
-      <c r="AG13" s="4"/>
+      <c r="U13" s="5"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="17"/>
+      <c r="AG13" s="17"/>
     </row>
     <row r="14" spans="3:33" ht="0.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I14" s="3"/>
@@ -1202,485 +1202,485 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="3:33" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="T15" s="9" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="T15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="U15" s="9"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
-      <c r="AG15" s="4"/>
+      <c r="U15" s="5"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="17"/>
     </row>
     <row r="16" spans="3:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="T16" s="9" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="T16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="U16" s="9"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4"/>
-      <c r="AG16" s="4"/>
+      <c r="U16" s="5"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+      <c r="AG16" s="17"/>
     </row>
     <row r="17" spans="3:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="T17" s="9" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="T17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="U17" s="9"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="4"/>
-      <c r="AG17" s="4"/>
+      <c r="U17" s="5"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="17"/>
+      <c r="AF17" s="17"/>
+      <c r="AG17" s="17"/>
     </row>
     <row r="18" spans="3:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="T18" s="9" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="T18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="U18" s="9"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="4"/>
-      <c r="AF18" s="4"/>
-      <c r="AG18" s="4"/>
+      <c r="U18" s="5"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+      <c r="AG18" s="17"/>
     </row>
     <row r="19" spans="3:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
     </row>
     <row r="20" spans="3:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
     </row>
     <row r="21" spans="3:33" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="22" spans="3:33" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="G22" s="12" t="s">
+      <c r="E22" s="9"/>
+      <c r="G22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12" t="s">
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12" t="s">
+      <c r="V22" s="9"/>
+      <c r="W22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="12" t="s">
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AB22" s="12"/>
-      <c r="AC22" s="19" t="s">
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="AD22" s="19"/>
-      <c r="AE22" s="19"/>
-      <c r="AF22" s="13" t="s">
+      <c r="AD22" s="16"/>
+      <c r="AE22" s="16"/>
+      <c r="AF22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AG22" s="13"/>
+      <c r="AG22" s="10"/>
     </row>
     <row r="23" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C23" s="2">
         <v>1</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="G23" s="14" t="s">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="G23" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="15" t="s">
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="V23" s="15"/>
-      <c r="W23" s="16">
+      <c r="V23" s="12"/>
+      <c r="W23" s="13">
         <v>1</v>
       </c>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="16"/>
-      <c r="AA23" s="17">
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="14">
         <v>1</v>
       </c>
-      <c r="AB23" s="17"/>
-      <c r="AC23" s="18">
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="15">
         <v>20</v>
       </c>
-      <c r="AD23" s="18"/>
-      <c r="AE23" s="18"/>
-      <c r="AF23" s="17">
+      <c r="AD23" s="15"/>
+      <c r="AE23" s="15"/>
+      <c r="AF23" s="14">
         <v>1</v>
       </c>
-      <c r="AG23" s="17"/>
+      <c r="AG23" s="14"/>
     </row>
     <row r="24" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AE25" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="8"/>
+    </row>
     <row r="26" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="X26" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y26" s="21"/>
-      <c r="Z26" s="21"/>
-      <c r="AA26" s="21"/>
-      <c r="AB26" s="21"/>
-      <c r="AC26" s="21"/>
-      <c r="AE26" s="22">
-        <v>1</v>
-      </c>
-      <c r="AF26" s="22"/>
-      <c r="AG26" s="22"/>
+      <c r="X26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="7"/>
+      <c r="AE26" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="8"/>
     </row>
     <row r="27" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="X27" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y27" s="21"/>
-      <c r="Z27" s="21"/>
-      <c r="AA27" s="21"/>
-      <c r="AB27" s="21"/>
-      <c r="AC27" s="21"/>
-      <c r="AE27" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="AF27" s="22"/>
-      <c r="AG27" s="22"/>
-    </row>
-    <row r="28" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="X28" s="21" t="s">
+      <c r="X27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Y28" s="21"/>
-      <c r="Z28" s="21"/>
-      <c r="AA28" s="21"/>
-      <c r="AB28" s="21"/>
-      <c r="AC28" s="21"/>
-      <c r="AE28" s="22">
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+      <c r="AC27" s="7"/>
+      <c r="AE27" s="8">
         <v>1.2</v>
       </c>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="22"/>
-    </row>
-    <row r="29" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="AF27" s="8"/>
+      <c r="AG27" s="8"/>
+    </row>
+    <row r="28" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+    </row>
     <row r="30" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C30" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
+      <c r="C30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
     </row>
     <row r="31" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C31" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="20"/>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
-      <c r="Y31" s="20"/>
-      <c r="Z31" s="20"/>
-      <c r="AA31" s="20"/>
-      <c r="AB31" s="20"/>
-      <c r="AC31" s="20"/>
-      <c r="AD31" s="20"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+      <c r="AA31" s="6"/>
+      <c r="AB31" s="6"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6"/>
     </row>
     <row r="32" spans="3:33" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="20"/>
-      <c r="X32" s="20"/>
-      <c r="Y32" s="20"/>
-      <c r="Z32" s="20"/>
-      <c r="AA32" s="20"/>
-      <c r="AB32" s="20"/>
-      <c r="AC32" s="20"/>
-      <c r="AD32" s="20"/>
+      <c r="C32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
     </row>
     <row r="33" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C33" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-    </row>
-    <row r="34" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C34" s="9" t="s">
+      <c r="C33" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="M35" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Z35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA35" s="5"/>
+    </row>
     <row r="36" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C36" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="M36" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Z36" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA36" s="9"/>
+      <c r="C36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="M36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
     </row>
     <row r="37" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C37" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="M37" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Z37" s="9"/>
-      <c r="AA37" s="9"/>
+      <c r="M37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
     </row>
     <row r="38" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M38" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Z38" s="9"/>
-      <c r="AA38" s="9"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
     </row>
     <row r="39" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="23"/>
-      <c r="R39" s="23"/>
-      <c r="S39" s="23"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="23"/>
-      <c r="V39" s="23"/>
-      <c r="W39" s="23"/>
-    </row>
-    <row r="40" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C40" s="9" t="s">
+      <c r="C39" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="Z40" s="9" t="s">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="Z39" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AA40" s="9"/>
-      <c r="AB40" s="9"/>
-      <c r="AC40" s="9"/>
-      <c r="AD40" s="9"/>
-      <c r="AE40" s="9"/>
-      <c r="AF40" s="9"/>
-    </row>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="5"/>
+      <c r="AC39" s="5"/>
+      <c r="AD39" s="5"/>
+      <c r="AE39" s="5"/>
+      <c r="AF39" s="5"/>
+    </row>
+    <row r="40" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="42" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="43" spans="3:32" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1705,67 +1705,8 @@
     <row r="62" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="63" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="64" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="Z40:AF40"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="M36:P36"/>
-    <mergeCell ref="Z36:AA38"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="M37:P37"/>
-    <mergeCell ref="M38:P39"/>
-    <mergeCell ref="Q39:W39"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:M30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:AD32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H33:O33"/>
-    <mergeCell ref="X26:AC26"/>
-    <mergeCell ref="AE26:AG26"/>
-    <mergeCell ref="X27:AC27"/>
-    <mergeCell ref="AE27:AG27"/>
-    <mergeCell ref="X28:AC28"/>
-    <mergeCell ref="AE28:AG28"/>
-    <mergeCell ref="W22:Z22"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="G23:T23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="W23:Z23"/>
-    <mergeCell ref="AA23:AB23"/>
-    <mergeCell ref="AC23:AE23"/>
-    <mergeCell ref="AF23:AG23"/>
-    <mergeCell ref="AC22:AE22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="G22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="I19:Q19"/>
-    <mergeCell ref="I20:Q20"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="I18:Q18"/>
-    <mergeCell ref="I12:Q12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="X13:AG13"/>
-    <mergeCell ref="X15:AG15"/>
-    <mergeCell ref="X16:AG16"/>
-    <mergeCell ref="X17:AG17"/>
-    <mergeCell ref="I17:Q17"/>
-    <mergeCell ref="I16:Q16"/>
-    <mergeCell ref="I15:Q15"/>
-    <mergeCell ref="I13:Q13"/>
     <mergeCell ref="X18:AG18"/>
     <mergeCell ref="C2:S3"/>
     <mergeCell ref="C4:S4"/>
@@ -1782,6 +1723,64 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="T12:U12"/>
     <mergeCell ref="X12:AG12"/>
+    <mergeCell ref="X13:AG13"/>
+    <mergeCell ref="X15:AG15"/>
+    <mergeCell ref="X16:AG16"/>
+    <mergeCell ref="X17:AG17"/>
+    <mergeCell ref="I17:Q17"/>
+    <mergeCell ref="I16:Q16"/>
+    <mergeCell ref="I15:Q15"/>
+    <mergeCell ref="I13:Q13"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="I18:Q18"/>
+    <mergeCell ref="I12:Q12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="G22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="I19:Q19"/>
+    <mergeCell ref="I20:Q20"/>
+    <mergeCell ref="W22:Z22"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="G23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:Z23"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="AC23:AE23"/>
+    <mergeCell ref="AF23:AG23"/>
+    <mergeCell ref="AC22:AE22"/>
+    <mergeCell ref="H32:O32"/>
+    <mergeCell ref="X25:AC25"/>
+    <mergeCell ref="AE25:AG25"/>
+    <mergeCell ref="X26:AC26"/>
+    <mergeCell ref="AE26:AG26"/>
+    <mergeCell ref="X27:AC27"/>
+    <mergeCell ref="AE27:AG27"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="Z39:AF39"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="Z35:AA37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="M36:P36"/>
+    <mergeCell ref="M37:P38"/>
+    <mergeCell ref="Q38:W38"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:M29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:AD31"/>
+    <mergeCell ref="C32:G32"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>